<commit_message>
this is new added code for rk...
</commit_message>
<xml_diff>
--- a/Externaldata/Salel_Of_Seed.xlsx
+++ b/Externaldata/Salel_Of_Seed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8DED0E-3BC5-4EFA-A4B2-BBB50F2B93C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB33B588-27F9-4308-BCE2-CB18A08EAA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>District</t>
   </si>
@@ -119,10 +119,13 @@
     <t>Ganjam</t>
   </si>
   <si>
-    <t>Verify</t>
-  </si>
-  <si>
-    <t>Successfully verify</t>
+    <t>Successfu</t>
+  </si>
+  <si>
+    <t>Not Verified</t>
+  </si>
+  <si>
+    <t>Successfully Verified</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -527,7 +530,7 @@
     <col min="1" max="1" customWidth="true" width="18.109375"/>
     <col min="2" max="2" customWidth="true" width="17.77734375"/>
     <col min="3" max="3" customWidth="true" width="15.21875"/>
-    <col min="4" max="4" customWidth="true" width="12.0"/>
+    <col min="4" max="4" customWidth="true" width="20.44140625"/>
     <col min="5" max="5" customWidth="true" width="18.5546875"/>
     <col min="6" max="6" customWidth="true" width="20.44140625"/>
     <col min="7" max="7" customWidth="true" width="13.77734375"/>
@@ -671,7 +674,7 @@
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="4" t="s">

</xml_diff>

<commit_message>
this is new code for changes
</commit_message>
<xml_diff>
--- a/Externaldata/Salel_Of_Seed.xlsx
+++ b/Externaldata/Salel_Of_Seed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CD49E5-C818-447A-AAB7-4B6252A51915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8480DAA7-6BB1-4097-8496-75BE11DE4E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>Ganjam</t>
   </si>
   <si>
-    <t>Succ</t>
+    <t>Successfully</t>
   </si>
   <si>
     <t>Successfully Verified</t>

</xml_diff>